<commit_message>
bicluster from FFIAF data
</commit_message>
<xml_diff>
--- a/output/moodle/bicluster/moodle-biconExprs.xlsx
+++ b/output/moodle/bicluster/moodle-biconExprs.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="moodle" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="moodle1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="moodle2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -13178,4 +13179,1165 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BD42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Flaw_Rule</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shamim_Rezaie  </t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bas_Brands  </t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Andrew_Nicols  </t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amaia_Anabitarte  </t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tim_Hunt  </t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Damyon_Wiese  </t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matt_Porritt  </t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tom_Dickman  </t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">David_Monllao  </t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ryan_Wyllie  </t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Marina_Glancy  </t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brendan_Heywood  </t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mark_Nelson  </t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sam_marshall  </t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mihail_Geshoski  </t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frederic_Massart  </t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Juan_Leyva  </t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simey_Lameze  </t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ankit_Agarwal  </t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">David_Mudrak  </t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cameron_Ball  </t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gthomas2  </t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilya_Tregubov  </t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jun_Pataleta  </t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John_Okely  </t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dan_Poltawski  </t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mark_Nielsen  </t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brendan_Anderson  </t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jean-Michel_Vedrine  </t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rossiani_Wijaya  </t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Colin_Chambers  </t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Petr_Skoda  </t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nobelium  </t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Andrew_Davis  </t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sam_Hemelryk  </t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James_McQuillan  </t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yuliya_Bozhko  </t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sam_Chaffee  </t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mayank_Gupa  </t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eloy_Lafuente_(stronk7)  </t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Andreas_Grabs  </t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dongsheng_Cai  </t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davo_Smith  </t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mikhail_Golenkov  </t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sara_Arjona  </t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Helen_Foster  </t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rajesh_Taneja  </t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">skodak  </t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eric_Merrill  </t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inaki  </t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tony_Levi  </t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>Eloy_Lafuente_(stronk7)</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">moodler  </t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">donal72  </t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fiedorow  </t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>javascript:S2201</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>javascript:S2259</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>javascript:S2583</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
+        <v>11</v>
+      </c>
+      <c r="K4" t="n">
+        <v>3</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>php:S836</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>javascript:S3403</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>9</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>php:S2201</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>php:S1848</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>5</v>
+      </c>
+      <c r="O8" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>php:S1656</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>2</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>php:S3923</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>php:S2964</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" t="n">
+        <v>11</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" t="n">
+        <v>8</v>
+      </c>
+      <c r="R11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Web:BoldAndItalicTagsCheck</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>21</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>javascript:S2757</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>javascript:S2819</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>php:S1763</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>2</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>13</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>javascript:S2873</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>javascript:S1143</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>javascript:UnreachableCode</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>php:S2053</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>php:S2068</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>2</v>
+      </c>
+      <c r="L20" t="n">
+        <v>3</v>
+      </c>
+      <c r="P20" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" t="n">
+        <v>15</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY20" t="n">
+        <v>2</v>
+      </c>
+      <c r="BA20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>javascript:S3981</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>javascript:S3785</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>16</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>php:S1764</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" t="n">
+        <v>2</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>php:S1862</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>javascript:S2137</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>javascript:DuplicatePropertyName</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Web:DoctypePresenceCheck</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Web:FieldsetWithoutLegendCheck</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>php:S4433</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>php:S2757</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Web:PageWithoutTitleCheck</t>
+        </is>
+      </c>
+      <c r="Q31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>javascript:S1656</t>
+        </is>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>php:S4830</t>
+        </is>
+      </c>
+      <c r="S33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY33" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC33" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Web:ImgWithoutAltCheck</t>
+        </is>
+      </c>
+      <c r="T34" t="n">
+        <v>1</v>
+      </c>
+      <c r="U34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>javascript:S905</t>
+        </is>
+      </c>
+      <c r="AE35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>javascript:S3812</t>
+        </is>
+      </c>
+      <c r="AG36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>javascript:S4043</t>
+        </is>
+      </c>
+      <c r="AG37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>php:S1145</t>
+        </is>
+      </c>
+      <c r="AG38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>php:S905</t>
+        </is>
+      </c>
+      <c r="AG39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Web:UnsupportedTagsInHtml5Check</t>
+        </is>
+      </c>
+      <c r="AG40" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI40" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Web:FrameWithoutTitleCheck</t>
+        </is>
+      </c>
+      <c r="AI41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>php:S4423</t>
+        </is>
+      </c>
+      <c r="BB42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>